<commit_message>
Data for Exercise 6.14.
</commit_message>
<xml_diff>
--- a/data/Exercise6.14.xlsx
+++ b/data/Exercise6.14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551C9CC3-42AE-4144-819F-8FA2F8DD0DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CFF06F-A6E3-4DBC-BEBA-E9AD231BDEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE44FEE3-665E-4A68-9D90-100DE89AFD07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE44FEE3-665E-4A68-9D90-100DE89AFD07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Factor1</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>x2</t>
+  </si>
+  <si>
+    <t>Rep</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4987A264-E7C1-4C24-B8AA-BA58FA148FA3}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,13 +446,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,13 +463,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -471,13 +480,16 @@
         <v>2</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -485,13 +497,16 @@
         <v>3</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -499,13 +514,16 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -516,10 +534,13 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -527,13 +548,16 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>-3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>2</v>
       </c>
@@ -541,13 +565,16 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>2</v>
       </c>
@@ -555,13 +582,16 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>-4</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>3</v>
       </c>
@@ -569,13 +599,16 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>-3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>3</v>
       </c>
@@ -583,13 +616,16 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>-4</v>
+      </c>
+      <c r="E11">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>3</v>
       </c>
@@ -597,13 +633,16 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>-11</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>3</v>
       </c>
@@ -611,9 +650,216 @@
         <v>4</v>
       </c>
       <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>-4</v>
+      </c>
+      <c r="E13">
         <v>-6</v>
       </c>
-      <c r="D13">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>-2</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>-11</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>-6</v>
+      </c>
+      <c r="E25">
         <v>6</v>
       </c>
     </row>

</xml_diff>